<commit_message>
Revert "	modified:   setup.py"
This reverts commit 8c3a917e4b6a00c420d1080f92ee01547eb1bd70.
</commit_message>
<xml_diff>
--- a/DuLieuThucHanh2_V1.xlsx
+++ b/DuLieuThucHanh2_V1.xlsx
@@ -461,52 +461,52 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dnr84hCD</t>
+          <t>eaVCpp4k</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sản phẩm 195</t>
+          <t>Sản phẩm 7</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>802</v>
+        <v>698</v>
       </c>
       <c r="D2" t="n">
-        <v>80000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>snekTYpB</t>
+          <t>pB3VWHKU</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sản phẩm 273</t>
+          <t>Sản phẩm 245</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>965</v>
+        <v>576</v>
       </c>
       <c r="D3" t="n">
-        <v>90000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>xzEkdccu</t>
+          <t>B9zqgfCg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sản phẩm 363</t>
+          <t>Sản phẩm 34</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>916</v>
+        <v>871</v>
       </c>
       <c r="D4" t="n">
         <v>60000</v>
@@ -515,52 +515,52 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DnoBTdUL</t>
+          <t>59Y7A3DL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sản phẩm 347</t>
+          <t>Sản phẩm 411</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>646</v>
+        <v>801</v>
       </c>
       <c r="D5" t="n">
-        <v>80000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KiqPnCCF</t>
+          <t>p5AUswTK</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sản phẩm 170</t>
+          <t>Sản phẩm 233</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>511</v>
+        <v>634</v>
       </c>
       <c r="D6" t="n">
-        <v>60000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kn8VVrj4</t>
+          <t>MW2ck7W2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sản phẩm 24</t>
+          <t>Sản phẩm 217</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>849</v>
+        <v>549</v>
       </c>
       <c r="D7" t="n">
         <v>50000</v>
@@ -569,268 +569,268 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>pdF7mEXA</t>
+          <t>tJDc5qjb</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sản phẩm 208</t>
+          <t>Sản phẩm 377</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>534</v>
+        <v>706</v>
       </c>
       <c r="D8" t="n">
-        <v>70000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5YN3SnVZ</t>
+          <t>Xpxsdggc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sản phẩm 461</t>
+          <t>Sản phẩm 413</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D9" t="n">
-        <v>50000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>XXiioG9g</t>
+          <t>8bj7aDuw</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sản phẩm 102</t>
+          <t>Sản phẩm 404</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>899</v>
+        <v>742</v>
       </c>
       <c r="D10" t="n">
-        <v>80000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>YFP3oDns</t>
+          <t>9MecYKm5</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sản phẩm 55</t>
+          <t>Sản phẩm 314</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>954</v>
+        <v>729</v>
       </c>
       <c r="D11" t="n">
-        <v>80000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>p5Ku7eJe</t>
+          <t>sFTeFDDs</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sản phẩm 341</t>
+          <t>Sản phẩm 152</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>659</v>
+        <v>917</v>
       </c>
       <c r="D12" t="n">
-        <v>70000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>gmUaNWL7</t>
+          <t>BuNRavG4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sản phẩm 493</t>
+          <t>Sản phẩm 468</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>762</v>
+        <v>868</v>
       </c>
       <c r="D13" t="n">
-        <v>90000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>YEZLSQzh</t>
+          <t>drmxoHBn</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sản phẩm 460</t>
+          <t>Sản phẩm 489</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>788</v>
+        <v>707</v>
       </c>
       <c r="D14" t="n">
-        <v>60000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>eFWTqEfW</t>
+          <t>5M6rbKpx</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sản phẩm 261</t>
+          <t>Sản phẩm 188</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>651</v>
+        <v>835</v>
       </c>
       <c r="D15" t="n">
-        <v>60000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>mpgX4Qsf</t>
+          <t>n57a2oqE</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sản phẩm 142</t>
+          <t>Sản phẩm 335</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>789</v>
+        <v>733</v>
       </c>
       <c r="D16" t="n">
-        <v>50000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ffKCVzYt</t>
+          <t>dfqfYNd5</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sản phẩm 388</t>
+          <t>Sản phẩm 489</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>670</v>
+        <v>836</v>
       </c>
       <c r="D17" t="n">
-        <v>70000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>UE5RC8qR</t>
+          <t>5MMKGfwz</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sản phẩm 214</t>
+          <t>Sản phẩm 472</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>662</v>
+        <v>980</v>
       </c>
       <c r="D18" t="n">
-        <v>70000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>jqXjzEjG</t>
+          <t>fEnPbbDj</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sản phẩm 300</t>
+          <t>Sản phẩm 356</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>674</v>
+        <v>514</v>
       </c>
       <c r="D19" t="n">
-        <v>80000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KZK7MCeW</t>
+          <t>337vwA8N</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sản phẩm 228</t>
+          <t>Sản phẩm 149</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>815</v>
+        <v>892</v>
       </c>
       <c r="D20" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MQSrNDAo</t>
+          <t>P57n8Ajo</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sản phẩm 17</t>
+          <t>Sản phẩm 350</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>712</v>
+        <v>985</v>
       </c>
       <c r="D21" t="n">
-        <v>80000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4RjWHNqv</t>
+          <t>DuuJZnhe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sản phẩm 70</t>
+          <t>Sản phẩm 62</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>704</v>
+        <v>904</v>
       </c>
       <c r="D22" t="n">
         <v>60000</v>
@@ -839,16 +839,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>nUtzQhrW</t>
+          <t>fSARNJqH</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sản phẩm 231</t>
+          <t>Sản phẩm 85</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>910</v>
+        <v>936</v>
       </c>
       <c r="D23" t="n">
         <v>60000</v>
@@ -857,34 +857,34 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>cGoivXHu</t>
+          <t>e9ynD6cs</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sản phẩm 119</t>
+          <t>Sản phẩm 10</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="D24" t="n">
-        <v>90000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>tKeBm5eA</t>
+          <t>kyLQTFkp</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sản phẩm 152</t>
+          <t>Sản phẩm 379</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>657</v>
+        <v>956</v>
       </c>
       <c r="D25" t="n">
         <v>70000</v>
@@ -893,142 +893,142 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3qqfYMWZ</t>
+          <t>pM8Vpe7S</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sản phẩm 480</t>
+          <t>Sản phẩm 287</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>874</v>
+        <v>585</v>
       </c>
       <c r="D26" t="n">
-        <v>80000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>syoNxQQY</t>
+          <t>swcb93H3</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sản phẩm 51</t>
+          <t>Sản phẩm 179</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>797</v>
+        <v>909</v>
       </c>
       <c r="D27" t="n">
-        <v>90000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Te5t94gk</t>
+          <t>tVA6EGmb</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sản phẩm 490</t>
+          <t>Sản phẩm 177</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>980</v>
+        <v>879</v>
       </c>
       <c r="D28" t="n">
-        <v>70000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>aJbncTyc</t>
+          <t>Vhc3rtgb</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sản phẩm 186</t>
+          <t>Sản phẩm 189</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>584</v>
+        <v>940</v>
       </c>
       <c r="D29" t="n">
-        <v>50000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BLJupGaW</t>
+          <t>PxkmkCDw</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sản phẩm 7</t>
+          <t>Sản phẩm 419</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>836</v>
+        <v>927</v>
       </c>
       <c r="D30" t="n">
-        <v>90000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>sCLD5d8X</t>
+          <t>kLK8NQzN</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sản phẩm 196</t>
+          <t>Sản phẩm 439</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>718</v>
+        <v>996</v>
       </c>
       <c r="D31" t="n">
-        <v>90000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5YMezPxE</t>
+          <t>RXUGytjR</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sản phẩm 50</t>
+          <t>Sản phẩm 338</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D32" t="n">
-        <v>60000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>rUCbWFJG</t>
+          <t>JXoUzHZb</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sản phẩm 310</t>
+          <t>Sản phẩm 278</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>764</v>
+        <v>789</v>
       </c>
       <c r="D33" t="n">
         <v>50000</v>
@@ -1037,34 +1037,34 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>8qRYt53Y</t>
+          <t>g3MF42Aa</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sản phẩm 200</t>
+          <t>Sản phẩm 284</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>704</v>
+        <v>640</v>
       </c>
       <c r="D34" t="n">
-        <v>50000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PWruxLGg</t>
+          <t>bYBeNJBy</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Sản phẩm 213</t>
+          <t>Sản phẩm 469</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>984</v>
+        <v>670</v>
       </c>
       <c r="D35" t="n">
         <v>80000</v>
@@ -1073,214 +1073,214 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>q97XmcTg</t>
+          <t>T64erj84</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sản phẩm 127</t>
+          <t>Sản phẩm 430</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>803</v>
+        <v>783</v>
       </c>
       <c r="D36" t="n">
-        <v>90000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mh8dmq5k</t>
+          <t>3we9qWBy</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sản phẩm 210</t>
+          <t>Sản phẩm 139</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="D37" t="n">
-        <v>50000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>94fCzfRX</t>
+          <t>Tb8BXVzo</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sản phẩm 254</t>
+          <t>Sản phẩm 332</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>837</v>
+        <v>929</v>
       </c>
       <c r="D38" t="n">
-        <v>60000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>dYuTxaK8</t>
+          <t>KVF4nPCa</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sản phẩm 456</t>
+          <t>Sản phẩm 192</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>676</v>
+        <v>872</v>
       </c>
       <c r="D39" t="n">
-        <v>80000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>3QwZaNGW</t>
+          <t>Le4xhR2M</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sản phẩm 477</t>
+          <t>Sản phẩm 153</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>860</v>
+        <v>960</v>
       </c>
       <c r="D40" t="n">
-        <v>90000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5jRoSAMA</t>
+          <t>VrsDBKge</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Sản phẩm 289</t>
+          <t>Sản phẩm 95</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>932</v>
+        <v>556</v>
       </c>
       <c r="D41" t="n">
-        <v>70000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CY5Zab6T</t>
+          <t>mVsEhsxn</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sản phẩm 499</t>
+          <t>Sản phẩm 341</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>532</v>
+        <v>653</v>
       </c>
       <c r="D42" t="n">
-        <v>80000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>RFQ6Bezj</t>
+          <t>NcuM3adV</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sản phẩm 155</t>
+          <t>Sản phẩm 38</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>932</v>
+        <v>634</v>
       </c>
       <c r="D43" t="n">
-        <v>80000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6dmmboTf</t>
+          <t>qUwDVwxe</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sản phẩm 378</t>
+          <t>Sản phẩm 99</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>782</v>
+        <v>948</v>
       </c>
       <c r="D44" t="n">
-        <v>50000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>7Td3fgQU</t>
+          <t>FUi3cNKK</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sản phẩm 56</t>
+          <t>Sản phẩm 425</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>766</v>
+        <v>958</v>
       </c>
       <c r="D45" t="n">
-        <v>50000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>EDrEKLc6</t>
+          <t>KgDRPj6F</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sản phẩm 462</t>
+          <t>Sản phẩm 259</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>576</v>
+        <v>974</v>
       </c>
       <c r="D46" t="n">
-        <v>90000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>4Ja7YhSE</t>
+          <t>spkndqjA</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sản phẩm 35</t>
+          <t>Sản phẩm 281</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>814</v>
+        <v>757</v>
       </c>
       <c r="D47" t="n">
         <v>60000</v>
@@ -1289,16 +1289,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>VohGqFbs</t>
+          <t>3MT6LwL7</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sản phẩm 232</t>
+          <t>Sản phẩm 105</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="D48" t="n">
         <v>50000</v>
@@ -1307,16 +1307,16 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>PzYXMe5i</t>
+          <t>noLRMdC9</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Sản phẩm 221</t>
+          <t>Sản phẩm 101</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>725</v>
+        <v>924</v>
       </c>
       <c r="D49" t="n">
         <v>50000</v>
@@ -1325,37 +1325,37 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7TCaLXZc</t>
+          <t>386HLd3J</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sản phẩm 292</t>
+          <t>Sản phẩm 131</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>687</v>
+        <v>895</v>
       </c>
       <c r="D50" t="n">
-        <v>90000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>nSuGAyge</t>
+          <t>KP32srJW</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sản phẩm 10</t>
+          <t>Sản phẩm 283</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>648</v>
+        <v>966</v>
       </c>
       <c r="D51" t="n">
-        <v>90000</v>
+        <v>80000</v>
       </c>
     </row>
   </sheetData>
@@ -1392,600 +1392,600 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Q9oeoDer</t>
+          <t>LuWTsx89</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Huỳnh Nguyệt Anh</t>
+          <t>Trương Quỳnh Thanh</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3Yt3dcYo</t>
+          <t>6z5AixNK</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dương Quỳnh Dung</t>
+          <t>Đỗ Thanh Ngân</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NN6uUXbh</t>
+          <t>ibJ9Qnup</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Huỳnh Trúc Vân</t>
+          <t>Ngô Kim Thoa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5mUbbBqE</t>
+          <t>ERob7HAD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hoàng Minh Loan</t>
+          <t>Vũ Nhan Hồng</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>m9SEa6iw</t>
+          <t>gFhdcNnq</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ngô Diệu Ngà</t>
+          <t>Phan Như Hảo</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>QRZHJtq2</t>
+          <t>MZP7SUYE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hoàng Xuân Hân</t>
+          <t>Võ Thiên Khánh</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Roip49Vj</t>
+          <t>dvr3UWih</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Vũ Phương Dung</t>
+          <t>Nguyễn Quỳnh Nhung</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ovB8eVzm</t>
+          <t>RJHcUEXK</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Huỳnh Thúy Minh</t>
+          <t>Trần Bảo Thoa</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>nZHAPD5k</t>
+          <t>fjT6e8jq</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vũ Hạnh My</t>
+          <t>Trần Ngọc Ðàn</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>P8Z9Ma9d</t>
+          <t>ZviKZXqi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Phạm Yên Nhi</t>
+          <t>Bùi Từ Dung</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>U7yHpQRE</t>
+          <t>bQKNzaxu</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lý Hương Lan</t>
+          <t>Đặng Yến Nhi</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UifBBUsX</t>
+          <t>3EQudp7v</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Đoàn Yến Loan</t>
+          <t>Trần Hải Vy</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>eQTCmd23</t>
+          <t>i2ysoCYs</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Đoàn Mỹ Trâm</t>
+          <t>Dương Thảo Quyên</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>dNrHzA7x</t>
+          <t>bB2i3oGs</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Đoàn Minh Đan</t>
+          <t>Lý Phương Nghi</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TJ9CCZrB</t>
+          <t>dEv8Ka4u</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Trần Kiều Nguyệt</t>
+          <t>Hoàng Thanh Thanh</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hfrp7yAc</t>
+          <t>48mERKph</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nguyễn Vân Thanh</t>
+          <t>Trương Thụy Khanh</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HtNW7yi7</t>
+          <t>M7VPwyXd</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lý Diễm Trang</t>
+          <t>Trần Thạch Thảo</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EwTEQUQ2</t>
+          <t>qXXmmfh8</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ngô Thanh Nhàn</t>
+          <t>Hồ Bảo Hà</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>rSvot5br</t>
+          <t>Kozet8SD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Đặng Như Mai</t>
+          <t>Phan Dạ Thi</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5tfWh3w5</t>
+          <t>h9XkvxqY</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Đoàn Xuân Hân</t>
+          <t>Hồ Ánh Lệ</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>QP8hEHs2</t>
+          <t>tiw3VN64</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Vũ Thanh Trúc</t>
+          <t>Bùi Thường Xuân</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>hwjeLxqT</t>
+          <t>5quvJ9Fy</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Huỳnh Minh Uyên</t>
+          <t>Lê Nguyệt Uyển</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>fg33vQ93</t>
+          <t>kzo5p7LQ</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Trần Mai Thảo</t>
+          <t>Hồ Ngọc Ái</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Yeq9wrKf</t>
+          <t>A3kHGgPy</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Bùi Tố Tâm</t>
+          <t>Đoàn Duy Hạnh</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>mzLyVnBp</t>
+          <t>nibocMEx</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Hoàng Thục Khuê</t>
+          <t>Phan Diễm Châu</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NajZ7Eqd</t>
+          <t>8pHrsPpF</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Hồ Bích Hạnh</t>
+          <t>Phan Tùng Linh</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>tvxxRZHk</t>
+          <t>iVnhGHPq</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lê Quỳnh Thơ</t>
+          <t>Bùi Dã Lan</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>X2kjr3Ry</t>
+          <t>Njt63EpY</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Hồ Mai Nhi</t>
+          <t>Lê Hải Phương</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>aiW2Xxky</t>
+          <t>dNhcvdHW</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Đỗ Bạch Yến</t>
+          <t>Đoàn Thy Khanh</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GqYFXFty</t>
+          <t>SfU44X4L</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Dương Diễm Uyên</t>
+          <t>Vũ Oanh Thơ</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>aGmrTRvG</t>
+          <t>NpkTuLRM</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ngô Loan Châu</t>
+          <t>Lý Song Thư</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>NXrEH2sN</t>
+          <t>BNmUipQc</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Trương Hồng Thư</t>
+          <t>Đỗ Lâm Nhi</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4pGiQGUC</t>
+          <t>P5jW88SR</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Phạm Kim Mai</t>
+          <t>Lý Phương Trà</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>pGY2ift4</t>
+          <t>tMQPyf8L</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Đoàn Hạnh Trang</t>
+          <t>Nguyễn Kiều Diễm</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GBNgotbX</t>
+          <t>KPcc6og6</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Đoàn Bảo Quyên</t>
+          <t>Trương Mai Linh</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>NVzNRyh8</t>
+          <t>iM7C6EFW</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Nguyễn Lam Hà</t>
+          <t>Phạm Tuyết Oanh</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Nk6vL2mV</t>
+          <t>VXSDRvgt</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Vũ Mỹ Huệ</t>
+          <t>Hồ Linh Lan</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>auFxbeJY</t>
+          <t>FdNSwmNN</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Phạm Kim Khanh</t>
+          <t>Lê Tịnh Như</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GnkfgLVA</t>
+          <t>4zsFmNqM</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Đặng Đan Thanh</t>
+          <t>Đoàn Thu Thảo</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TCFMy8FH</t>
+          <t>aNaesdsL</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Đỗ Mỹ Nhi</t>
+          <t>Dương Ánh Ngọc</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Hx7FXUSZ</t>
+          <t>cgrCPhLy</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Lý Như Quân</t>
+          <t>Huỳnh Nguyệt Cát</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pXGEKNW7</t>
+          <t>KpxJpNoj</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Huỳnh Thụy Du</t>
+          <t>Phạm Thanh Mai</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>moCToVLD</t>
+          <t>chbQPuSW</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Phan Vi Quyên</t>
+          <t>Phạm Vân Ngọc</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>rceH8aLi</t>
+          <t>hWUoSi5c</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Huỳnh Tố Quyên</t>
+          <t>Lê Hải San</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>XL6NRPD4</t>
+          <t>tQQSiyFt</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Phan Kim Loan</t>
+          <t>Vũ Minh Duyên</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>nMwujjgi</t>
+          <t>wWajQXhR</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Lê Tú Anh</t>
+          <t>Hoàng Ngọc Hà</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>hrbaihNf</t>
+          <t>MABHRoPm</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Võ Hạnh Nhơn</t>
+          <t>Ngô Lan Vy</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>qeAfQuUd</t>
+          <t>tu5qsKiL</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Nguyễn Ánh Lệ</t>
+          <t>Đỗ Hoàng Cúc</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>VnAp28Jx</t>
+          <t>SKyyP9YE</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Đỗ Tùy Linh</t>
+          <t>Ngô Minh Châu</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>b6Cv7eRW</t>
+          <t>QodG2d8B</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Hoàng Hồng Bạch Thảo</t>
+          <t>Hồ Thanh Trang</t>
         </is>
       </c>
     </row>
@@ -2023,600 +2023,600 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>m6qtfVPz</t>
+          <t>QDmiAxAJ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fg33vQ93</t>
+          <t>fjT6e8jq</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3pBKTZiN</t>
+          <t>a7NHwBSU</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UifBBUsX</t>
+          <t>Kozet8SD</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Xsv9THSp</t>
+          <t>XYshNRXG</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EwTEQUQ2</t>
+          <t>ZviKZXqi</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HYH39J5G</t>
+          <t>UKHdLCFf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>UifBBUsX</t>
+          <t>LuWTsx89</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>46XTg7xT</t>
+          <t>ZeyQe6zq</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pXGEKNW7</t>
+          <t>ibJ9Qnup</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>87RgmVts</t>
+          <t>Dox5QUev</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>QP8hEHs2</t>
+          <t>tMQPyf8L</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DTdV5mv4</t>
+          <t>n2pArq4X</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>nMwujjgi</t>
+          <t>ZviKZXqi</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DcEprWA3</t>
+          <t>4fecnZmG</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TJ9CCZrB</t>
+          <t>LuWTsx89</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>gY79VGiS</t>
+          <t>o8RkNcvJ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ovB8eVzm</t>
+          <t>M7VPwyXd</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>r3rAtkST</t>
+          <t>7U2NdADK</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>NajZ7Eqd</t>
+          <t>M7VPwyXd</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>f5QTJR2H</t>
+          <t>XPZwp8bF</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>nZHAPD5k</t>
+          <t>gFhdcNnq</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cXVXqyoK</t>
+          <t>MPTaDeiv</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>aiW2Xxky</t>
+          <t>6z5AixNK</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6F2cYMEz</t>
+          <t>sETND7dG</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>rSvot5br</t>
+          <t>FdNSwmNN</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>K8ovb3QN</t>
+          <t>DryGBxPU</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NXrEH2sN</t>
+          <t>tQQSiyFt</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>yMPvF8BV</t>
+          <t>Efaz6ZJ2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>hwjeLxqT</t>
+          <t>h9XkvxqY</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5259dPob</t>
+          <t>sfnoWJ3z</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>b6Cv7eRW</t>
+          <t>tQQSiyFt</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HQL6bk3Z</t>
+          <t>VNCCgD6s</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>hwjeLxqT</t>
+          <t>qXXmmfh8</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BUYVr8St</t>
+          <t>p2e9XJdB</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>pGY2ift4</t>
+          <t>KpxJpNoj</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AXdgC4Co</t>
+          <t>iooLnRMs</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>fg33vQ93</t>
+          <t>ibJ9Qnup</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>QEnk2NhU</t>
+          <t>VpyoQTNv</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>GqYFXFty</t>
+          <t>KPcc6og6</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>S5oQVACN</t>
+          <t>HGzGBXnf</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HtNW7yi7</t>
+          <t>Njt63EpY</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Hfrtr7cL</t>
+          <t>32WGa6v5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Hx7FXUSZ</t>
+          <t>KPcc6og6</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6qRXFtMu</t>
+          <t>JGLaU5U4</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>auFxbeJY</t>
+          <t>cgrCPhLy</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>sMZBw7WE</t>
+          <t>VPwb7PmN</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NVzNRyh8</t>
+          <t>h9XkvxqY</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>WqbahBkp</t>
+          <t>6567Wv8s</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Hx7FXUSZ</t>
+          <t>wWajQXhR</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>mRKY7Lzy</t>
+          <t>CEP2Gmeu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NN6uUXbh</t>
+          <t>6z5AixNK</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>hoobfs32</t>
+          <t>a94PXoZc</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>b6Cv7eRW</t>
+          <t>dNhcvdHW</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Gy9XU36r</t>
+          <t>qEPQcQ2H</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>m9SEa6iw</t>
+          <t>gFhdcNnq</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>kdWfDBes</t>
+          <t>JvKbDxS5</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>mzLyVnBp</t>
+          <t>KpxJpNoj</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>H3SSFcxm</t>
+          <t>3N2PPZRx</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TCFMy8FH</t>
+          <t>48mERKph</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>JkhA2rPd</t>
+          <t>AeMUBuvw</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>auFxbeJY</t>
+          <t>gFhdcNnq</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6Y8UfvEy</t>
+          <t>44YipJgh</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>dNrHzA7x</t>
+          <t>iM7C6EFW</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>erVxQY6b</t>
+          <t>YAsAtMjm</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>nMwujjgi</t>
+          <t>MZP7SUYE</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PwniyAbK</t>
+          <t>7nSVLiJx</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>mzLyVnBp</t>
+          <t>KPcc6og6</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R6MBGUpK</t>
+          <t>LvPWMp6p</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>mzLyVnBp</t>
+          <t>8pHrsPpF</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>8f5zaHih</t>
+          <t>DDYVCry3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QP8hEHs2</t>
+          <t>bB2i3oGs</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>jMbB7Rpz</t>
+          <t>CU5UXuyj</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5mUbbBqE</t>
+          <t>QodG2d8B</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>eoEa4SLD</t>
+          <t>W7X4TS8S</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Roip49Vj</t>
+          <t>dNhcvdHW</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>oe3uABFM</t>
+          <t>YmjzGBnx</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>m9SEa6iw</t>
+          <t>48mERKph</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>8j69dPen</t>
+          <t>rVZ2BuWD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8Z9Ma9d</t>
+          <t>ZviKZXqi</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Gk3Ty2Lu</t>
+          <t>7g4joY46</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>EwTEQUQ2</t>
+          <t>5quvJ9Fy</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>XAwkVcZv</t>
+          <t>GghvSGZq</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>m9SEa6iw</t>
+          <t>4zsFmNqM</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>8WYZRTJP</t>
+          <t>AYjsRk2r</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5mUbbBqE</t>
+          <t>5quvJ9Fy</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>LEWauVSg</t>
+          <t>4474cJsj</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TCFMy8FH</t>
+          <t>iM7C6EFW</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>8V3zvF4F</t>
+          <t>BejNtCFH</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>aGmrTRvG</t>
+          <t>tMQPyf8L</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ETAHKRBW</t>
+          <t>G4ryhW6Y</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8Z9Ma9d</t>
+          <t>3EQudp7v</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>eFw97kaz</t>
+          <t>pHHePBZn</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>HtNW7yi7</t>
+          <t>KpxJpNoj</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hmAR5WBD</t>
+          <t>7nmfAbGE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>HtNW7yi7</t>
+          <t>dNhcvdHW</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>8FiscUMH</t>
+          <t>5RgxF5XH</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>NXrEH2sN</t>
+          <t>3EQudp7v</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DsjMs8P2</t>
+          <t>3sri4Ck5</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>XL6NRPD4</t>
+          <t>tMQPyf8L</t>
         </is>
       </c>
     </row>
@@ -2659,252 +2659,252 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>QEnk2NhU</t>
+          <t>AYjsRk2r</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rUCbWFJG</t>
+          <t>kLK8NQzN</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>QEnk2NhU</t>
+          <t>44YipJgh</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>rUCbWFJG</t>
+          <t>KgDRPj6F</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Xsv9THSp</t>
+          <t>XYshNRXG</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7TCaLXZc</t>
+          <t>g3MF42Aa</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HYH39J5G</t>
+          <t>UKHdLCFf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>nSuGAyge</t>
+          <t>Xpxsdggc</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>46XTg7xT</t>
+          <t>44YipJgh</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5YN3SnVZ</t>
+          <t>KgDRPj6F</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>87RgmVts</t>
+          <t>Dox5QUev</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PzYXMe5i</t>
+          <t>qUwDVwxe</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DTdV5mv4</t>
+          <t>n2pArq4X</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MQSrNDAo</t>
+          <t>NcuM3adV</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>eoEa4SLD</t>
+          <t>4fecnZmG</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5YN3SnVZ</t>
+          <t>drmxoHBn</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>gY79VGiS</t>
+          <t>o8RkNcvJ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5YN3SnVZ</t>
+          <t>JXoUzHZb</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>r3rAtkST</t>
+          <t>7U2NdADK</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Te5t94gk</t>
+          <t>8bj7aDuw</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>f5QTJR2H</t>
+          <t>XPZwp8bF</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>8qRYt53Y</t>
+          <t>DuuJZnhe</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cXVXqyoK</t>
+          <t>MPTaDeiv</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>gmUaNWL7</t>
+          <t>PxkmkCDw</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6F2cYMEz</t>
+          <t>sETND7dG</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>xzEkdccu</t>
+          <t>Xpxsdggc</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>K8ovb3QN</t>
+          <t>DryGBxPU</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CY5Zab6T</t>
+          <t>KP32srJW</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>yMPvF8BV</t>
+          <t>Efaz6ZJ2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RFQ6Bezj</t>
+          <t>KVF4nPCa</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5259dPob</t>
+          <t>sfnoWJ3z</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>snekTYpB</t>
+          <t>mVsEhsxn</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HQL6bk3Z</t>
+          <t>VNCCgD6s</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>8qRYt53Y</t>
+          <t>eaVCpp4k</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -2914,496 +2914,496 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BUYVr8St</t>
+          <t>p2e9XJdB</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>nSuGAyge</t>
+          <t>P57n8Ajo</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AXdgC4Co</t>
+          <t>iooLnRMs</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>nSuGAyge</t>
+          <t>spkndqjA</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>QEnk2NhU</t>
+          <t>VpyoQTNv</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>rUCbWFJG</t>
+          <t>KP32srJW</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>S5oQVACN</t>
+          <t>HGzGBXnf</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>XXiioG9g</t>
+          <t>noLRMdC9</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Hfrtr7cL</t>
+          <t>32WGa6v5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>pdF7mEXA</t>
+          <t>dfqfYNd5</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>QEnk2NhU</t>
+          <t>JGLaU5U4</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>rUCbWFJG</t>
+          <t>Le4xhR2M</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>sMZBw7WE</t>
+          <t>VPwb7PmN</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>YEZLSQzh</t>
+          <t>p5AUswTK</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>WqbahBkp</t>
+          <t>6567Wv8s</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4RjWHNqv</t>
+          <t>Xpxsdggc</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>mRKY7Lzy</t>
+          <t>CEP2Gmeu</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>UE5RC8qR</t>
+          <t>KgDRPj6F</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>hoobfs32</t>
+          <t>a94PXoZc</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Kn8VVrj4</t>
+          <t>DuuJZnhe</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Gy9XU36r</t>
+          <t>qEPQcQ2H</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PzYXMe5i</t>
+          <t>kLK8NQzN</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>kdWfDBes</t>
+          <t>JvKbDxS5</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ffKCVzYt</t>
+          <t>n57a2oqE</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>H3SSFcxm</t>
+          <t>3N2PPZRx</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kn8VVrj4</t>
+          <t>3MT6LwL7</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>JkhA2rPd</t>
+          <t>AeMUBuvw</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cGoivXHu</t>
+          <t>3MT6LwL7</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6Y8UfvEy</t>
+          <t>44YipJgh</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>94fCzfRX</t>
+          <t>KgDRPj6F</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>erVxQY6b</t>
+          <t>YAsAtMjm</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>7TCaLXZc</t>
+          <t>NcuM3adV</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>12</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PwniyAbK</t>
+          <t>7nSVLiJx</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5jRoSAMA</t>
+          <t>e9ynD6cs</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>R6MBGUpK</t>
+          <t>LvPWMp6p</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>gmUaNWL7</t>
+          <t>386HLd3J</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>8f5zaHih</t>
+          <t>DDYVCry3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Kn8VVrj4</t>
+          <t>59Y7A3DL</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>jMbB7Rpz</t>
+          <t>CU5UXuyj</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>jqXjzEjG</t>
+          <t>kyLQTFkp</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>eoEa4SLD</t>
+          <t>W7X4TS8S</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5YN3SnVZ</t>
+          <t>JXoUzHZb</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>oe3uABFM</t>
+          <t>YmjzGBnx</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>UE5RC8qR</t>
+          <t>P57n8Ajo</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>8j69dPen</t>
+          <t>rVZ2BuWD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Te5t94gk</t>
+          <t>n57a2oqE</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Gk3Ty2Lu</t>
+          <t>7g4joY46</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>snekTYpB</t>
+          <t>8bj7aDuw</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>XAwkVcZv</t>
+          <t>GghvSGZq</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>EDrEKLc6</t>
+          <t>kyLQTFkp</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>8WYZRTJP</t>
+          <t>AYjsRk2r</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CY5Zab6T</t>
+          <t>kLK8NQzN</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>46XTg7xT</t>
+          <t>4474cJsj</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5YN3SnVZ</t>
+          <t>9MecYKm5</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>8V3zvF4F</t>
+          <t>BejNtCFH</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6dmmboTf</t>
+          <t>pM8Vpe7S</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ETAHKRBW</t>
+          <t>G4ryhW6Y</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4RjWHNqv</t>
+          <t>8bj7aDuw</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>eFw97kaz</t>
+          <t>pHHePBZn</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>YFP3oDns</t>
+          <t>JXoUzHZb</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hmAR5WBD</t>
+          <t>7nmfAbGE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>rUCbWFJG</t>
+          <t>DuuJZnhe</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>8FiscUMH</t>
+          <t>5RgxF5XH</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>RFQ6Bezj</t>
+          <t>NcuM3adV</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DsjMs8P2</t>
+          <t>3sri4Ck5</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>PWruxLGg</t>
+          <t>pB3VWHKU</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>